<commit_message>
finish first round leetcode
</commit_message>
<xml_diff>
--- a/奋斗日程.xlsx
+++ b/奋斗日程.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FightingForOffer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8D13D6-B370-4DB0-AB99-ADB9FFD1DB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C0D7B5-5A72-40B6-9061-3B0D044D81C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="750" windowWidth="21600" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12450" yWindow="1200" windowWidth="21600" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>Leetcode</t>
   </si>
@@ -2205,7 +2205,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>53、最大子序列和---贪心难、连续要体现（简单）
+      <t xml:space="preserve">53、最大子序列和---贪心难、连续要体现（简单）
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>动态规划---编辑距离篇</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 392、判断子序列---双指针、动规（简单）</t>
     </r>
     <r>
@@ -2230,6 +2253,60 @@
         <scheme val="minor"/>
       </rPr>
       <t>115、不同的子序列---从递归想到动规（困难）</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">583、两个字符串的删除操作---递推中两个都要删除（中等）
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>72、编辑距离---自底向上、自上而下（困难）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>动态规划---回文</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+647、回文子串---动规、双指针（中等）
+516、最长回文子序列---（中等）</t>
     </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -2697,11 +2774,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3432,12 +3509,20 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44413</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>44414</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>